<commit_message>
Added an ability to extract simple formulae from a spreadsheet
</commit_message>
<xml_diff>
--- a/doc/ExampleSpreadsheet.xlsx
+++ b/doc/ExampleSpreadsheet.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
+    <sheet name="FormulaeTypes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,19 +20,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Sharing</t>
+  </si>
+  <si>
+    <t>Array (single)</t>
+  </si>
+  <si>
+    <t>Arraying (multiple)</t>
+  </si>
+  <si>
+    <t>Arrayed (multiple)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,13 +89,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -439,4 +482,98 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>COSH(2*PI())</f>
+        <v>267.74676148374817</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">COSH(2*PI())</f>
+        <v>267.74676148374817</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>267.74676148374817</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="array" ref="B5">B1:B4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="array" ref="B6:B8">IF(B3:B5=8,"Eight","Not Eight")</f>
+        <v>Not Eight</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Not Eight</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Not Eight</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>